<commit_message>
more static page changes
</commit_message>
<xml_diff>
--- a/blakearchive/static/html/StaticPages.xlsx
+++ b/blakearchive/static/html/StaticPages.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26812"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Blake Drive/REDESIGN/Static Pages/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7920" yWindow="1720" windowWidth="32840" windowHeight="20320" tabRatio="500"/>
+    <workbookView xWindow="15120" yWindow="1220" windowWidth="34820" windowHeight="25840" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="86">
   <si>
     <t>Main page item</t>
   </si>
@@ -206,9 +201,6 @@
     <t>Needs updating</t>
   </si>
   <si>
-    <t>This would replace the "Blake Archive in the Context of IATH/CDLA page." It may not be necessary.</t>
-  </si>
-  <si>
     <t>We may or may not decide to create a new tour</t>
   </si>
   <si>
@@ -264,6 +256,27 @@
   </si>
   <si>
     <t>Needs updating (mentions Inote, for instance)</t>
+  </si>
+  <si>
+    <t>All past updates should be linked to this page</t>
+  </si>
+  <si>
+    <t>All internal links in past update pages need to be checked (and some added; older updates don't have links to the published works like new updates do). Formats are also not standardized; we should consider whether we want to do this.</t>
+  </si>
+  <si>
+    <t>Recent and Forthcoming Presentations</t>
+  </si>
+  <si>
+    <t>articlesindex.html</t>
+  </si>
+  <si>
+    <t>generalbib.html</t>
+  </si>
+  <si>
+    <t>specificbib.html</t>
+  </si>
+  <si>
+    <t>This would replace the "Blake Archive in the Context of IATH/CDLA" page. It may not be necessary.</t>
   </si>
 </sst>
 </file>
@@ -935,24 +948,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F56"/>
+  <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="26.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33.5" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="50.83203125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="45.83203125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="57.33203125" style="2" customWidth="1"/>
     <col min="7" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="6" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="6" customFormat="1" ht="18">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -966,13 +979,13 @@
         <v>3</v>
       </c>
       <c r="E1" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="F1" s="8" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" s="6" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6" s="6" customFormat="1" ht="18">
       <c r="A2" s="7"/>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -980,9 +993,9 @@
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
     </row>
-    <row r="3" spans="1:6" s="6" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" s="6" customFormat="1" ht="18">
       <c r="A3" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
@@ -990,38 +1003,38 @@
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B5" s="1" t="s">
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="9"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1" t="s">
         <v>74</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="9"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>75</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>25</v>
       </c>
       <c r="C7" s="11"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="B8" s="10"/>
       <c r="C8" s="11"/>
     </row>
-    <row r="9" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="18">
       <c r="A9" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B9" s="10"/>
       <c r="C9" s="11"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
         <v>4</v>
       </c>
@@ -1029,18 +1042,24 @@
         <v>11</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="60">
       <c r="C12" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="C13" s="5" t="s">
         <v>5</v>
       </c>
@@ -1048,7 +1067,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6">
       <c r="C14" s="5" t="s">
         <v>7</v>
       </c>
@@ -1056,11 +1075,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6">
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6">
       <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
@@ -1070,7 +1089,7 @@
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6">
       <c r="C17" s="5" t="s">
         <v>13</v>
       </c>
@@ -1078,7 +1097,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6">
       <c r="C18" s="4" t="s">
         <v>14</v>
       </c>
@@ -1086,7 +1105,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6">
       <c r="C19" s="4" t="s">
         <v>15</v>
       </c>
@@ -1094,7 +1113,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" ht="30">
       <c r="C20" s="4" t="s">
         <v>16</v>
       </c>
@@ -1102,11 +1121,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6">
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
@@ -1116,23 +1135,23 @@
       <c r="C22" s="5"/>
       <c r="D22" s="3"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6">
       <c r="C23" s="4" t="s">
         <v>22</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="C24" s="4" t="s">
         <v>23</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="30">
       <c r="C25" s="4" t="s">
         <v>24</v>
       </c>
@@ -1143,11 +1162,11 @@
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6">
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
@@ -1157,7 +1176,7 @@
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6">
       <c r="C28" s="4" t="s">
         <v>28</v>
       </c>
@@ -1165,32 +1184,32 @@
         <v>37</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="30">
       <c r="C29" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D29" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F29" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="F29" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:6">
       <c r="C30" s="4" t="s">
         <v>29</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
       <c r="C31" s="4" t="s">
         <v>48</v>
       </c>
@@ -1198,7 +1217,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6">
       <c r="C32" s="4" t="s">
         <v>52</v>
       </c>
@@ -1206,10 +1225,10 @@
         <v>53</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
       <c r="C33" s="4" t="s">
         <v>31</v>
       </c>
@@ -1217,7 +1236,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" ht="30">
       <c r="C34" s="4" t="s">
         <v>32</v>
       </c>
@@ -1225,148 +1244,161 @@
         <v>39</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6">
       <c r="C35" s="4" t="s">
         <v>35</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="30">
       <c r="C36" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="C37" s="4" t="s">
         <v>36</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="C37" s="4" t="s">
-        <v>70</v>
       </c>
       <c r="D37" s="4" t="s">
         <v>25</v>
       </c>
       <c r="F37" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="30">
+      <c r="C38" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="30">
+      <c r="C39" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="C42" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F42" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C38" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C39" s="4"/>
-      <c r="D39" s="4"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B40" s="1" t="s">
+    <row r="43" spans="1:6">
+      <c r="C43" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D43" s="4" t="s">
         <v>42</v>
-      </c>
-      <c r="C40" s="5"/>
-      <c r="D40" s="5"/>
-      <c r="E40" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C41" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C42" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C43" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>41</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C44" s="4"/>
-      <c r="D44" s="4"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46" s="1" t="s">
+    <row r="44" spans="1:6">
+      <c r="C44" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B47" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E46" s="2" t="s">
+      <c r="E47" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A48" s="1" t="s">
+    <row r="49" spans="1:6" ht="30">
+      <c r="A49" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E48" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A50" s="1" t="s">
+      <c r="E49" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B51" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A52" s="1" t="s">
+    <row r="53" spans="1:6">
+      <c r="A53" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B53" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="64" x14ac:dyDescent="0.2">
-      <c r="F54" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" ht="64" x14ac:dyDescent="0.2">
-      <c r="F56" s="2" t="s">
-        <v>78</v>
+    <row r="55" spans="1:6" ht="45">
+      <c r="F55" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="45">
+      <c r="F57" s="2" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>